<commit_message>
Edited Power System Spreadsheet
</commit_message>
<xml_diff>
--- a/ME/power_system.xlsx
+++ b/ME/power_system.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\StormDrainRobot\ME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E40E660-39A8-4FFE-BBE8-46416FBF478E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9D51C1-FFD1-46B7-9348-50498B27F1B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{654665DF-210C-496C-AD7F-CE8AF87E9115}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{654665DF-210C-496C-AD7F-CE8AF87E9115}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery Monitoring" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="90">
   <si>
     <t>Battery Nominal Voltage</t>
   </si>
@@ -297,6 +297,15 @@
   </si>
   <si>
     <t>OE(Enable Pin)</t>
+  </si>
+  <si>
+    <t>Vout</t>
+  </si>
+  <si>
+    <t>Runtime(hr)</t>
+  </si>
+  <si>
+    <t>Battery Standby Voltage</t>
   </si>
 </sst>
 </file>
@@ -385,10 +394,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -413,13 +422,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>73039</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>487940</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>138545</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -802,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D1F36D-4D94-4A0E-9DA4-02DA4ECFE1B0}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,7 +825,7 @@
     <col min="4" max="4" width="13.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="7" t="s">
         <v>60</v>
@@ -829,7 +838,7 @@
       </c>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>50</v>
       </c>
@@ -837,150 +846,184 @@
         <v>14.2</v>
       </c>
       <c r="C2" s="5">
-        <f>(B2*$B$11)/($B$10+$B$11)</f>
+        <f>(B2*$B$12)/($B$11+$B$12)</f>
         <v>1.9586206896551723</v>
       </c>
       <c r="D2" s="6">
-        <f>(1/$B$9)*C2</f>
+        <f>(1/$B$10)*C2</f>
         <v>62675.862068965514</v>
       </c>
       <c r="E2" s="6">
-        <f>D2-D3</f>
+        <f>D2-D4</f>
         <v>6179.310344827587</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="4">
+        <v>13.8</v>
+      </c>
+      <c r="C3" s="5">
+        <f>(B3*$B$12)/($B$11+$B$12)</f>
+        <v>1.903448275862069</v>
+      </c>
+      <c r="D3" s="6">
+        <f>(1/$B$10)*C3</f>
+        <v>60910.34482758621</v>
+      </c>
+      <c r="E3" s="6">
+        <f>D3-D5</f>
+        <v>7944.8275862068986</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B4" s="4">
         <v>12.8</v>
       </c>
-      <c r="C3" s="5">
-        <f t="shared" ref="C3:C5" si="0">(B3*$B$11)/($B$10+$B$11)</f>
+      <c r="C4" s="5">
+        <f t="shared" ref="C4:C6" si="0">(B4*$B$12)/($B$11+$B$12)</f>
         <v>1.7655172413793103</v>
       </c>
-      <c r="D3" s="6">
-        <f t="shared" ref="D3:D5" si="1">(1/$B$9)*C3</f>
+      <c r="D4" s="6">
+        <f t="shared" ref="D4:D6" si="1">(1/$B$10)*C4</f>
         <v>56496.551724137928</v>
       </c>
-      <c r="E3" s="6">
-        <f t="shared" ref="E3:E4" si="2">D3-D4</f>
+      <c r="E4" s="6">
+        <f t="shared" ref="E4:E5" si="2">D4-D5</f>
         <v>3531.0344827586159</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="H4">
+        <v>1.738</v>
+      </c>
+      <c r="I4">
+        <f>(B11+B12)*H4/B12</f>
+        <v>12.6005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B5" s="4">
         <v>12</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C5" s="5">
         <f t="shared" si="0"/>
         <v>1.6551724137931034</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D5" s="6">
         <f t="shared" si="1"/>
         <v>52965.517241379312</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E5" s="6">
         <f t="shared" si="2"/>
         <v>2206.8965517241377</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B6" s="4">
         <v>11.5</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C6" s="5">
         <f t="shared" si="0"/>
         <v>1.5862068965517242</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D6" s="6">
         <f t="shared" si="1"/>
         <v>50758.620689655174</v>
       </c>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>57</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>2.048</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>58</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>59</v>
       </c>
-      <c r="B8">
-        <f>2^B7</f>
+      <c r="B9">
+        <f>2^B8</f>
         <v>65536</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>63</v>
       </c>
-      <c r="B9">
-        <f>B6/B8</f>
+      <c r="B10">
+        <f>B7/B9</f>
         <v>3.1250000000000001E-5</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" s="3">
+        <f>B10*1000</f>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>61</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>30000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>62</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>4800</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>64</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>14.5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>56</v>
       </c>
     </row>
@@ -995,15 +1038,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F429EF87-7522-4814-9EDC-46F679FC0812}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="69" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="207.42578125" bestFit="1" customWidth="1"/>
@@ -1032,13 +1077,13 @@
       <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="10"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B2">
@@ -1171,7 +1216,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B7">
@@ -1264,9 +1309,6 @@
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
       <c r="C10">
         <v>8.6999999999999993</v>
       </c>
@@ -1275,14 +1317,14 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>4</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1311,7 +1353,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B12">
@@ -1339,7 +1381,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>32</v>
       </c>
       <c r="H13">
@@ -1352,13 +1394,22 @@
         <v>47</v>
       </c>
     </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+    </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
+      <c r="F16">
+        <f>20/G16</f>
+        <v>3.3002755730103464</v>
+      </c>
       <c r="G16">
         <f>SUM(G2:G12)</f>
-        <v>26.060099999999998</v>
+        <v>6.0601000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1375,7 +1426,7 @@
       </c>
       <c r="G18">
         <f>G17-G16</f>
-        <v>3.9399000000000015</v>
+        <v>23.939900000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1397,7 +1448,7 @@
   <dimension ref="A2:K14"/>
   <sheetViews>
     <sheetView zoomScale="116" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,7 +1686,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>